<commit_message>
fixed typo in starter sheet
</commit_message>
<xml_diff>
--- a/docs/unit1/4_graphing_numsolver/(Starter-Workbook)-Class-Graphing-and-Solver.xlsx
+++ b/docs/unit1/4_graphing_numsolver/(Starter-Workbook)-Class-Graphing-and-Solver.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/python_projects/content/docs/unit1/4_graphing_numsolver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92C8FF5-4212-EE48-B810-50C52EA8B91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29645E6A-FD60-4948-9CEC-7DAE84CEA410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21660" yWindow="740" windowWidth="33900" windowHeight="25380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -658,8 +658,8 @@
       <xdr:rowOff>19660</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3344698" cy="326628"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -848,7 +848,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -1128,7 +1128,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>2. Use the </a:t>
+            <a:t>3. Use the </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
@@ -42555,7 +42555,7 @@
   <dimension ref="A9:F46"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -42631,7 +42631,7 @@
         <v>-2</v>
       </c>
       <c r="C18" s="6">
-        <f>$C$11*B18^4+$C$12*B18^3+$C$13*B18^2+$C$14*B18+$C$15</f>
+        <f t="shared" ref="C18:C38" si="0">$C$11*B18^4+$C$12*B18^3+$C$13*B18^2+$C$14*B18+$C$15</f>
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -42640,7 +42640,7 @@
         <v>-1.8</v>
       </c>
       <c r="C19" s="6">
-        <f>$C$11*B19^4+$C$12*B19^3+$C$13*B19^2+$C$14*B19+$C$15</f>
+        <f t="shared" si="0"/>
         <v>1.3776000000000015</v>
       </c>
     </row>
@@ -42649,7 +42649,7 @@
         <v>-1.6</v>
       </c>
       <c r="C20" s="6">
-        <f>$C$11*B20^4+$C$12*B20^3+$C$13*B20^2+$C$14*B20+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-0.52639999999999854</v>
       </c>
     </row>
@@ -42658,7 +42658,7 @@
         <v>-1.4</v>
       </c>
       <c r="C21" s="6">
-        <f>$C$11*B21^4+$C$12*B21^3+$C$13*B21^2+$C$14*B21+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-1.4384000000000001</v>
       </c>
     </row>
@@ -42667,7 +42667,7 @@
         <v>-1.2</v>
       </c>
       <c r="C22" s="6">
-        <f>$C$11*B22^4+$C$12*B22^3+$C$13*B22^2+$C$14*B22+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-1.6464000000000003</v>
       </c>
     </row>
@@ -42676,7 +42676,7 @@
         <v>-1</v>
       </c>
       <c r="C23" s="6">
-        <f>$C$11*B23^4+$C$12*B23^3+$C$13*B23^2+$C$14*B23+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-1.4</v>
       </c>
     </row>
@@ -42685,7 +42685,7 @@
         <v>-0.8</v>
       </c>
       <c r="C24" s="6">
-        <f>$C$11*B24^4+$C$12*B24^3+$C$13*B24^2+$C$14*B24+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-0.91040000000000021</v>
       </c>
     </row>
@@ -42694,7 +42694,7 @@
         <v>-0.6</v>
       </c>
       <c r="C25" s="6">
-        <f>$C$11*B25^4+$C$12*B25^3+$C$13*B25^2+$C$14*B25+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-0.35040000000000016</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -42707,7 +42707,7 @@
         <v>-0.4</v>
       </c>
       <c r="C26" s="6">
-        <f>$C$11*B26^4+$C$12*B26^3+$C$13*B26^2+$C$14*B26+$C$15</f>
+        <f t="shared" si="0"/>
         <v>0.1455999999999999</v>
       </c>
       <c r="E26" s="7" t="s">
@@ -42720,7 +42720,7 @@
         <v>-0.2</v>
       </c>
       <c r="C27" s="6">
-        <f>$C$11*B27^4+$C$12*B27^3+$C$13*B27^2+$C$14*B27+$C$15</f>
+        <f t="shared" si="0"/>
         <v>0.48159999999999997</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -42733,7 +42733,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="6">
-        <f>$C$11*B28^4+$C$12*B28^3+$C$13*B28^2+$C$14*B28+$C$15</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -42746,7 +42746,7 @@
         <v>0.2</v>
       </c>
       <c r="C29" s="6">
-        <f>$C$11*B29^4+$C$12*B29^3+$C$13*B29^2+$C$14*B29+$C$15</f>
+        <f t="shared" si="0"/>
         <v>0.48159999999999997</v>
       </c>
     </row>
@@ -42755,7 +42755,7 @@
         <v>0.4</v>
       </c>
       <c r="C30" s="6">
-        <f>$C$11*B30^4+$C$12*B30^3+$C$13*B30^2+$C$14*B30+$C$15</f>
+        <f t="shared" si="0"/>
         <v>0.1455999999999999</v>
       </c>
     </row>
@@ -42764,7 +42764,7 @@
         <v>0.6</v>
       </c>
       <c r="C31" s="6">
-        <f>$C$11*B31^4+$C$12*B31^3+$C$13*B31^2+$C$14*B31+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-0.35040000000000016</v>
       </c>
     </row>
@@ -42773,7 +42773,7 @@
         <v>0.8</v>
       </c>
       <c r="C32" s="6">
-        <f>$C$11*B32^4+$C$12*B32^3+$C$13*B32^2+$C$14*B32+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-0.91040000000000021</v>
       </c>
     </row>
@@ -42782,7 +42782,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="6">
-        <f>$C$11*B33^4+$C$12*B33^3+$C$13*B33^2+$C$14*B33+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-1.4</v>
       </c>
     </row>
@@ -42791,7 +42791,7 @@
         <v>1.2</v>
       </c>
       <c r="C34" s="6">
-        <f>$C$11*B34^4+$C$12*B34^3+$C$13*B34^2+$C$14*B34+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-1.6464000000000003</v>
       </c>
       <c r="E34" s="7" t="s">
@@ -42804,7 +42804,7 @@
         <v>1.4</v>
       </c>
       <c r="C35" s="6">
-        <f>$C$11*B35^4+$C$12*B35^3+$C$13*B35^2+$C$14*B35+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-1.4384000000000001</v>
       </c>
       <c r="E35" s="7" t="s">
@@ -42817,7 +42817,7 @@
         <v>1.6</v>
       </c>
       <c r="C36" s="6">
-        <f>$C$11*B36^4+$C$12*B36^3+$C$13*B36^2+$C$14*B36+$C$15</f>
+        <f t="shared" si="0"/>
         <v>-0.52639999999999854</v>
       </c>
     </row>
@@ -42826,7 +42826,7 @@
         <v>1.8</v>
       </c>
       <c r="C37" s="6">
-        <f>$C$11*B37^4+$C$12*B37^3+$C$13*B37^2+$C$14*B37+$C$15</f>
+        <f t="shared" si="0"/>
         <v>1.3776000000000015</v>
       </c>
     </row>
@@ -42835,7 +42835,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="6">
-        <f>$C$11*B38^4+$C$12*B38^3+$C$13*B38^2+$C$14*B38+$C$15</f>
+        <f t="shared" si="0"/>
         <v>4.5999999999999996</v>
       </c>
     </row>

</xml_diff>